<commit_message>
add json file & excel (forget last time
Calendar Q: set year in [2000, 2100], maybe need modified.
</commit_message>
<xml_diff>
--- a/TestCaseExcelAndDoc/练习1_2_万年历佣金测试用例.xlsx
+++ b/TestCaseExcelAndDoc/练习1_2_万年历佣金测试用例.xlsx
@@ -1,25 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sTern/Downloads/EE_Study/3.5/软件测试/project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7B2C4FF-4ADA-B842-9832-5873619C5435}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED77FD2E-E103-EF43-91D9-9745AB744189}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="280" yWindow="460" windowWidth="19120" windowHeight="16420" xr2:uid="{6525DCF9-0BF7-0343-A4EC-E7C228D98259}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="19120" windowHeight="16420" xr2:uid="{6525DCF9-0BF7-0343-A4EC-E7C228D98259}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -740,7 +745,7 @@
   <dimension ref="A1:I133"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="94" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2398,7 +2403,7 @@
         <v>46</v>
       </c>
       <c r="G102">
-        <f t="shared" ref="G101:G121" si="0">SUM(D102*25,E102*30,F102*45)</f>
+        <f t="shared" ref="G102:G120" si="0">SUM(D102*25,E102*30,F102*45)</f>
         <v>3295</v>
       </c>
       <c r="H102">
@@ -2605,31 +2610,6 @@
         <v>626</v>
       </c>
     </row>
-    <row r="111" spans="1:9">
-      <c r="C111">
-        <v>12</v>
-      </c>
-      <c r="D111">
-        <v>40</v>
-      </c>
-      <c r="E111">
-        <v>40</v>
-      </c>
-      <c r="F111">
-        <v>46</v>
-      </c>
-      <c r="G111">
-        <f t="shared" si="0"/>
-        <v>4270</v>
-      </c>
-      <c r="H111">
-        <v>20</v>
-      </c>
-      <c r="I111">
-        <f t="shared" si="1"/>
-        <v>854</v>
-      </c>
-    </row>
     <row r="112" spans="1:9">
       <c r="C112">
         <v>13</v>
@@ -2774,31 +2754,6 @@
       <c r="I117">
         <f t="shared" si="1"/>
         <v>458</v>
-      </c>
-    </row>
-    <row r="118" spans="3:9">
-      <c r="C118">
-        <v>19</v>
-      </c>
-      <c r="D118">
-        <v>40</v>
-      </c>
-      <c r="E118">
-        <v>40</v>
-      </c>
-      <c r="F118">
-        <v>46</v>
-      </c>
-      <c r="G118">
-        <f t="shared" si="0"/>
-        <v>4270</v>
-      </c>
-      <c r="H118">
-        <v>20</v>
-      </c>
-      <c r="I118">
-        <f t="shared" si="1"/>
-        <v>854</v>
       </c>
     </row>
     <row r="119" spans="3:9">

</xml_diff>